<commit_message>
patchwork package with the most recent version is broken, replaced it with grid arrange
</commit_message>
<xml_diff>
--- a/docs/sqi_data_checking.xlsx
+++ b/docs/sqi_data_checking.xlsx
@@ -6369,8 +6369,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -6398,6 +6398,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:OldForms" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6491,6 +6492,13 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OldForms" ma:index="27" nillable="true" ma:displayName="Old Forms " ma:format="Dropdown" ma:internalName="OldForms">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -6644,7 +6652,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EE0CC0-5EE1-44FF-BE88-519CDFFB0936}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E91EB1D-1F78-45A0-804E-6289794B5D28}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>